<commit_message>
bulk density data dealt with
brought in and combined into a summary data frame which is saved as a
csv and prints an image comparing the methods

# output products:
# soilbulkdensity_processed.csv : bulk density summary CSV
# BDmethodcomparison.png: compares the results from the truth bar
method (july 2013) with the bulk density ring method (nov 2014)
</commit_message>
<xml_diff>
--- a/Soil-Data-Raw-R/Soil-Data-RawFolders/Bulk Density/NCD-bulkdensity-adilson.xlsx
+++ b/Soil-Data-Raw-R/Soil-Data-RawFolders/Bulk Density/NCD-bulkdensity-adilson.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5325" yWindow="0" windowWidth="21840" windowHeight="13740" tabRatio="500"/>
+    <workbookView xWindow="260" yWindow="4100" windowWidth="16060" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -133,11 +133,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -222,7 +222,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="113">
+  <cellStyleXfs count="143">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -336,8 +336,38 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -372,7 +402,6 @@
     <xf numFmtId="2" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -393,7 +422,78 @@
     <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="113">
+  <cellStyles count="143">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -450,62 +550,21 @@
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink seguido" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
@@ -955,21 +1014,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A98" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="A201" sqref="A201"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="36.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.625" style="17" customWidth="1"/>
-    <col min="4" max="5" width="13.625" style="7" customWidth="1"/>
-    <col min="6" max="7" width="13.625" style="2" customWidth="1"/>
-    <col min="8" max="16384" width="10.875" style="2"/>
+    <col min="3" max="3" width="13.6640625" style="17" customWidth="1"/>
+    <col min="4" max="5" width="13.6640625" style="7" customWidth="1"/>
+    <col min="6" max="7" width="13.6640625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1">
@@ -2149,7 +2208,7 @@
         <f t="shared" si="1"/>
         <v>472.23</v>
       </c>
-      <c r="F53" s="29" t="s">
+      <c r="F53" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G53" s="20" t="s">
@@ -2174,7 +2233,7 @@
         <f t="shared" si="1"/>
         <v>424.53000000000003</v>
       </c>
-      <c r="F54" s="29" t="s">
+      <c r="F54" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G54" s="20" t="s">
@@ -2199,7 +2258,7 @@
         <f t="shared" si="1"/>
         <v>477.13</v>
       </c>
-      <c r="F55" s="29" t="s">
+      <c r="F55" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G55" s="20" t="s">
@@ -2224,7 +2283,7 @@
         <f t="shared" si="1"/>
         <v>152.53</v>
       </c>
-      <c r="F56" s="29" t="s">
+      <c r="F56" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G56" s="20" t="s">
@@ -2249,7 +2308,7 @@
         <f t="shared" si="1"/>
         <v>500.43</v>
       </c>
-      <c r="F57" s="29" t="s">
+      <c r="F57" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G57" s="20" t="s">
@@ -2274,7 +2333,7 @@
         <f t="shared" si="1"/>
         <v>471.83</v>
       </c>
-      <c r="F58" s="29" t="s">
+      <c r="F58" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G58" s="20" t="s">
@@ -2299,7 +2358,7 @@
         <f t="shared" si="1"/>
         <v>467.33</v>
       </c>
-      <c r="F59" s="29" t="s">
+      <c r="F59" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G59" s="20" t="s">
@@ -2324,7 +2383,7 @@
         <f t="shared" si="1"/>
         <v>516.92999999999995</v>
       </c>
-      <c r="F60" s="29" t="s">
+      <c r="F60" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G60" s="20" t="s">
@@ -2349,7 +2408,7 @@
         <f t="shared" si="1"/>
         <v>483.63</v>
       </c>
-      <c r="F61" s="29" t="s">
+      <c r="F61" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G61" s="20" t="s">
@@ -2374,7 +2433,7 @@
         <f t="shared" si="1"/>
         <v>515.92999999999995</v>
       </c>
-      <c r="F62" s="29" t="s">
+      <c r="F62" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G62" s="20" t="s">
@@ -2399,7 +2458,7 @@
         <f t="shared" si="1"/>
         <v>479.93</v>
       </c>
-      <c r="F63" s="29" t="s">
+      <c r="F63" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G63" s="20" t="s">
@@ -2424,7 +2483,7 @@
         <f t="shared" si="1"/>
         <v>507.43</v>
       </c>
-      <c r="F64" s="29" t="s">
+      <c r="F64" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G64" s="20" t="s">
@@ -2449,7 +2508,7 @@
         <f t="shared" si="1"/>
         <v>492.73</v>
       </c>
-      <c r="F65" s="29" t="s">
+      <c r="F65" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G65" s="20" t="s">
@@ -2521,7 +2580,7 @@
         <f t="shared" ref="E68:E102" si="5">D68-C68</f>
         <v>473.23</v>
       </c>
-      <c r="F68" s="29" t="s">
+      <c r="F68" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G68" s="20" t="s">
@@ -2546,7 +2605,7 @@
         <f t="shared" si="5"/>
         <v>406.33</v>
       </c>
-      <c r="F69" s="29" t="s">
+      <c r="F69" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G69" s="20" t="s">
@@ -2571,7 +2630,7 @@
         <f t="shared" si="5"/>
         <v>441.63</v>
       </c>
-      <c r="F70" s="29" t="s">
+      <c r="F70" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G70" s="20" t="s">
@@ -2596,7 +2655,7 @@
         <f t="shared" si="5"/>
         <v>449.83</v>
       </c>
-      <c r="F71" s="29" t="s">
+      <c r="F71" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G71" s="20" t="s">
@@ -2621,7 +2680,7 @@
         <f t="shared" si="5"/>
         <v>428.13</v>
       </c>
-      <c r="F72" s="29" t="s">
+      <c r="F72" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G72" s="20" t="s">
@@ -2646,7 +2705,7 @@
         <f t="shared" si="5"/>
         <v>457.33</v>
       </c>
-      <c r="F73" s="29" t="s">
+      <c r="F73" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G73" s="20" t="s">
@@ -2671,7 +2730,7 @@
         <f t="shared" si="5"/>
         <v>455.13</v>
       </c>
-      <c r="F74" s="29" t="s">
+      <c r="F74" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G74" s="20" t="s">
@@ -2696,7 +2755,7 @@
         <f t="shared" si="5"/>
         <v>466.93</v>
       </c>
-      <c r="F75" s="29" t="s">
+      <c r="F75" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G75" s="20" t="s">
@@ -2721,7 +2780,7 @@
         <f t="shared" si="5"/>
         <v>365.93</v>
       </c>
-      <c r="F76" s="29" t="s">
+      <c r="F76" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G76" s="20" t="s">
@@ -2746,7 +2805,7 @@
         <f t="shared" si="5"/>
         <v>461.43</v>
       </c>
-      <c r="F77" s="29" t="s">
+      <c r="F77" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G77" s="20" t="s">
@@ -2771,7 +2830,7 @@
         <f t="shared" si="5"/>
         <v>463.73</v>
       </c>
-      <c r="F78" s="29" t="s">
+      <c r="F78" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G78" s="20" t="s">
@@ -2796,7 +2855,7 @@
         <f t="shared" si="5"/>
         <v>380.63</v>
       </c>
-      <c r="F79" s="29" t="s">
+      <c r="F79" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G79" s="20" t="s">
@@ -2821,7 +2880,7 @@
         <f t="shared" si="5"/>
         <v>427.13</v>
       </c>
-      <c r="F80" s="29" t="s">
+      <c r="F80" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G80" s="20" t="s">
@@ -2846,7 +2905,7 @@
         <f t="shared" si="5"/>
         <v>407.53000000000003</v>
       </c>
-      <c r="F81" s="29" t="s">
+      <c r="F81" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G81" s="20" t="s">
@@ -2871,7 +2930,7 @@
         <f t="shared" si="5"/>
         <v>451.93</v>
       </c>
-      <c r="F82" s="29" t="s">
+      <c r="F82" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G82" s="20" t="s">
@@ -2896,7 +2955,7 @@
         <f t="shared" si="5"/>
         <v>358.73</v>
       </c>
-      <c r="F83" s="29" t="s">
+      <c r="F83" s="28" t="s">
         <v>33</v>
       </c>
       <c r="G83" s="20" t="s">
@@ -2968,7 +3027,7 @@
         <f t="shared" si="5"/>
         <v>394.83</v>
       </c>
-      <c r="F86" s="28" t="s">
+      <c r="F86" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G86" s="20" t="s">
@@ -2993,7 +3052,7 @@
         <f t="shared" si="5"/>
         <v>499.22999999999996</v>
       </c>
-      <c r="F87" s="28" t="s">
+      <c r="F87" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G87" s="20" t="s">
@@ -3018,7 +3077,7 @@
         <f t="shared" si="5"/>
         <v>441.63</v>
       </c>
-      <c r="F88" s="28" t="s">
+      <c r="F88" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G88" s="20" t="s">
@@ -3043,7 +3102,7 @@
         <f t="shared" si="5"/>
         <v>496.53000000000003</v>
       </c>
-      <c r="F89" s="28" t="s">
+      <c r="F89" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G89" s="20" t="s">
@@ -3068,7 +3127,7 @@
         <f t="shared" si="5"/>
         <v>520.7299999999999</v>
       </c>
-      <c r="F90" s="28" t="s">
+      <c r="F90" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G90" s="20" t="s">
@@ -3093,7 +3152,7 @@
         <f t="shared" si="5"/>
         <v>472.23</v>
       </c>
-      <c r="F91" s="28" t="s">
+      <c r="F91" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G91" s="20" t="s">
@@ -3118,7 +3177,7 @@
         <f t="shared" si="5"/>
         <v>478.33</v>
       </c>
-      <c r="F92" s="28" t="s">
+      <c r="F92" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G92" s="20" t="s">
@@ -3143,7 +3202,7 @@
         <f t="shared" si="5"/>
         <v>527.82999999999993</v>
       </c>
-      <c r="F93" s="28" t="s">
+      <c r="F93" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G93" s="20" t="s">
@@ -3168,7 +3227,7 @@
         <f t="shared" si="5"/>
         <v>486.73</v>
       </c>
-      <c r="F94" s="28" t="s">
+      <c r="F94" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G94" s="20" t="s">
@@ -3193,7 +3252,7 @@
         <f t="shared" si="5"/>
         <v>527.2299999999999</v>
       </c>
-      <c r="F95" s="28" t="s">
+      <c r="F95" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G95" s="20" t="s">
@@ -3218,7 +3277,7 @@
         <f t="shared" si="5"/>
         <v>497.73</v>
       </c>
-      <c r="F96" s="28" t="s">
+      <c r="F96" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G96" s="20" t="s">
@@ -3243,7 +3302,7 @@
         <f t="shared" si="5"/>
         <v>454.63</v>
       </c>
-      <c r="F97" s="28" t="s">
+      <c r="F97" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G97" s="20" t="s">
@@ -3268,7 +3327,7 @@
         <f t="shared" si="5"/>
         <v>462.23</v>
       </c>
-      <c r="F98" s="28" t="s">
+      <c r="F98" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G98" s="20" t="s">
@@ -3293,7 +3352,7 @@
         <f t="shared" si="5"/>
         <v>528.92999999999995</v>
       </c>
-      <c r="F99" s="28" t="s">
+      <c r="F99" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G99" s="20" t="s">
@@ -3318,7 +3377,7 @@
         <f t="shared" si="5"/>
         <v>508.43</v>
       </c>
-      <c r="F100" s="28" t="s">
+      <c r="F100" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G100" s="20" t="s">
@@ -3343,7 +3402,7 @@
         <f t="shared" si="5"/>
         <v>496.53000000000003</v>
       </c>
-      <c r="F101" s="28" t="s">
+      <c r="F101" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G101" s="20" t="s">
@@ -3368,7 +3427,7 @@
         <f t="shared" si="5"/>
         <v>484.63</v>
       </c>
-      <c r="F102" s="28" t="s">
+      <c r="F102" s="27" t="s">
         <v>33</v>
       </c>
       <c r="G102" s="20" t="s">
@@ -3433,7 +3492,7 @@
         <f>$B$6</f>
         <v>4.753333333333333</v>
       </c>
-      <c r="D105" s="30">
+      <c r="D105" s="29">
         <v>284.10000000000002</v>
       </c>
       <c r="E105" s="7">
@@ -3443,7 +3502,7 @@
       <c r="F105" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G105" s="26">
+      <c r="G105" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -3458,7 +3517,7 @@
         <f t="shared" ref="C106:C125" si="8">$B$6</f>
         <v>4.753333333333333</v>
       </c>
-      <c r="D106" s="30">
+      <c r="D106" s="29">
         <v>281.5</v>
       </c>
       <c r="E106" s="7">
@@ -3468,7 +3527,7 @@
       <c r="F106" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G106" s="26">
+      <c r="G106" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -3483,7 +3542,7 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D107" s="30">
+      <c r="D107" s="29">
         <v>232.1</v>
       </c>
       <c r="E107" s="7">
@@ -3493,7 +3552,7 @@
       <c r="F107" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G107" s="26">
+      <c r="G107" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -3508,7 +3567,7 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D108" s="30">
+      <c r="D108" s="29">
         <v>333.4</v>
       </c>
       <c r="E108" s="7">
@@ -3518,7 +3577,7 @@
       <c r="F108" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G108" s="26">
+      <c r="G108" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -3533,7 +3592,7 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D109" s="30">
+      <c r="D109" s="29">
         <v>311.7</v>
       </c>
       <c r="E109" s="7">
@@ -3543,7 +3602,7 @@
       <c r="F109" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G109" s="26">
+      <c r="G109" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -3558,7 +3617,7 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D110" s="30">
+      <c r="D110" s="29">
         <v>286.39999999999998</v>
       </c>
       <c r="E110" s="7">
@@ -3568,7 +3627,7 @@
       <c r="F110" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G110" s="26">
+      <c r="G110" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -3583,7 +3642,7 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D111" s="30">
+      <c r="D111" s="29">
         <v>350.8</v>
       </c>
       <c r="E111" s="7">
@@ -3593,7 +3652,7 @@
       <c r="F111" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G111" s="26">
+      <c r="G111" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -3608,7 +3667,7 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D112" s="30">
+      <c r="D112" s="29">
         <v>337.2</v>
       </c>
       <c r="E112" s="7">
@@ -3618,7 +3677,7 @@
       <c r="F112" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G112" s="26">
+      <c r="G112" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -3633,7 +3692,7 @@
         <f>$B$6</f>
         <v>4.753333333333333</v>
       </c>
-      <c r="D113" s="30">
+      <c r="D113" s="29">
         <v>433.2</v>
       </c>
       <c r="E113" s="7">
@@ -3643,7 +3702,7 @@
       <c r="F113" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G113" s="26">
+      <c r="G113" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -3658,7 +3717,7 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D114" s="30">
+      <c r="D114" s="29">
         <v>272.39999999999998</v>
       </c>
       <c r="E114" s="7">
@@ -3668,7 +3727,7 @@
       <c r="F114" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G114" s="26">
+      <c r="G114" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -3683,7 +3742,7 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D115" s="30">
+      <c r="D115" s="29">
         <v>313.60000000000002</v>
       </c>
       <c r="E115" s="7">
@@ -3693,7 +3752,7 @@
       <c r="F115" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G115" s="26">
+      <c r="G115" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -3708,7 +3767,7 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D116" s="30">
+      <c r="D116" s="29">
         <v>324.8</v>
       </c>
       <c r="E116" s="7">
@@ -3718,7 +3777,7 @@
       <c r="F116" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G116" s="26">
+      <c r="G116" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -3733,7 +3792,7 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D117" s="30">
+      <c r="D117" s="29">
         <v>423.1</v>
       </c>
       <c r="E117" s="7">
@@ -3743,7 +3802,7 @@
       <c r="F117" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G117" s="26">
+      <c r="G117" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -3758,7 +3817,7 @@
         <f>$B$6</f>
         <v>4.753333333333333</v>
       </c>
-      <c r="D118" s="30">
+      <c r="D118" s="29">
         <v>337.6</v>
       </c>
       <c r="E118" s="7">
@@ -3768,7 +3827,7 @@
       <c r="F118" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G118" s="26">
+      <c r="G118" s="25">
         <v>41313</v>
       </c>
       <c r="H118" s="20"/>
@@ -3802,7 +3861,7 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D119" s="30">
+      <c r="D119" s="29">
         <v>394.2</v>
       </c>
       <c r="E119" s="7">
@@ -3812,7 +3871,7 @@
       <c r="F119" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G119" s="26">
+      <c r="G119" s="25">
         <v>41313</v>
       </c>
       <c r="H119" s="20"/>
@@ -3846,7 +3905,7 @@
         <f>$B$6</f>
         <v>4.753333333333333</v>
       </c>
-      <c r="D120" s="30">
+      <c r="D120" s="29">
         <v>235.7</v>
       </c>
       <c r="E120" s="7">
@@ -3856,7 +3915,7 @@
       <c r="F120" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G120" s="26">
+      <c r="G120" s="25">
         <v>41313</v>
       </c>
       <c r="H120" s="20"/>
@@ -3890,7 +3949,7 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D121" s="30">
+      <c r="D121" s="29">
         <v>324.8</v>
       </c>
       <c r="E121" s="7">
@@ -3900,7 +3959,7 @@
       <c r="F121" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G121" s="26">
+      <c r="G121" s="25">
         <v>41313</v>
       </c>
       <c r="H121" s="20"/>
@@ -3934,7 +3993,7 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D122" s="30">
+      <c r="D122" s="29">
         <v>302.89999999999998</v>
       </c>
       <c r="E122" s="7">
@@ -3944,7 +4003,7 @@
       <c r="F122" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G122" s="26">
+      <c r="G122" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -3959,7 +4018,7 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D123" s="30">
+      <c r="D123" s="29">
         <v>351</v>
       </c>
       <c r="E123" s="7">
@@ -3969,7 +4028,7 @@
       <c r="F123" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G123" s="26">
+      <c r="G123" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -3984,7 +4043,7 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D124" s="30">
+      <c r="D124" s="29">
         <v>263.39999999999998</v>
       </c>
       <c r="E124" s="7">
@@ -3994,7 +4053,7 @@
       <c r="F124" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G124" s="26">
+      <c r="G124" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -4009,15 +4068,11 @@
         <f t="shared" si="8"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D125" s="30"/>
-      <c r="E125" s="7">
-        <f t="shared" si="9"/>
-        <v>-4.753333333333333</v>
-      </c>
+      <c r="D125" s="29"/>
       <c r="F125" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G125" s="26">
+      <c r="G125" s="25">
         <v>41313</v>
       </c>
     </row>
@@ -4030,7 +4085,7 @@
       <c r="D126" s="15"/>
       <c r="E126" s="15">
         <f>SUM(E105:E125)</f>
-        <v>6294.08</v>
+        <v>6298.833333333333</v>
       </c>
       <c r="F126" s="14"/>
       <c r="G126" s="14"/>
@@ -4079,17 +4134,17 @@
         <f>$B$6</f>
         <v>4.753333333333333</v>
       </c>
-      <c r="D128" s="30">
+      <c r="D128" s="29">
         <v>407.4</v>
       </c>
       <c r="E128" s="7">
         <f t="shared" ref="E128:E148" si="10">D128-C128</f>
         <v>402.64666666666665</v>
       </c>
-      <c r="F128" s="29" t="s">
+      <c r="F128" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G128" s="27">
+      <c r="G128" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4104,17 +4159,17 @@
         <f t="shared" ref="C129:C148" si="11">$B$6</f>
         <v>4.753333333333333</v>
       </c>
-      <c r="D129" s="30">
+      <c r="D129" s="29">
         <v>425.2</v>
       </c>
       <c r="E129" s="7">
         <f t="shared" si="10"/>
         <v>420.44666666666666</v>
       </c>
-      <c r="F129" s="29" t="s">
+      <c r="F129" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G129" s="27">
+      <c r="G129" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4129,17 +4184,17 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D130" s="30">
+      <c r="D130" s="29">
         <v>354.6</v>
       </c>
       <c r="E130" s="7">
         <f t="shared" si="10"/>
         <v>349.84666666666669</v>
       </c>
-      <c r="F130" s="29" t="s">
+      <c r="F130" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G130" s="27">
+      <c r="G130" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4154,17 +4209,17 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D131" s="30">
+      <c r="D131" s="29">
         <v>494.9</v>
       </c>
       <c r="E131" s="7">
         <f t="shared" si="10"/>
         <v>490.14666666666665</v>
       </c>
-      <c r="F131" s="29" t="s">
+      <c r="F131" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G131" s="27">
+      <c r="G131" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4179,17 +4234,17 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D132" s="30">
+      <c r="D132" s="29">
         <v>400.6</v>
       </c>
       <c r="E132" s="7">
         <f t="shared" si="10"/>
         <v>395.84666666666669</v>
       </c>
-      <c r="F132" s="29" t="s">
+      <c r="F132" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G132" s="27">
+      <c r="G132" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4204,17 +4259,17 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D133" s="30">
+      <c r="D133" s="29">
         <v>269.60000000000002</v>
       </c>
       <c r="E133" s="7">
         <f t="shared" si="10"/>
         <v>264.84666666666669</v>
       </c>
-      <c r="F133" s="29" t="s">
+      <c r="F133" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G133" s="27">
+      <c r="G133" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4229,17 +4284,17 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D134" s="30">
+      <c r="D134" s="29">
         <v>399.7</v>
       </c>
       <c r="E134" s="7">
         <f t="shared" si="10"/>
         <v>394.94666666666666</v>
       </c>
-      <c r="F134" s="29" t="s">
+      <c r="F134" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G134" s="27">
+      <c r="G134" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4254,17 +4309,17 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D135" s="30">
+      <c r="D135" s="29">
         <v>238.9</v>
       </c>
       <c r="E135" s="7">
         <f t="shared" si="10"/>
         <v>234.14666666666668</v>
       </c>
-      <c r="F135" s="29" t="s">
+      <c r="F135" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G135" s="27">
+      <c r="G135" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4279,17 +4334,17 @@
         <f>$B$6</f>
         <v>4.753333333333333</v>
       </c>
-      <c r="D136" s="30">
+      <c r="D136" s="29">
         <v>317.60000000000002</v>
       </c>
       <c r="E136" s="7">
         <f t="shared" si="10"/>
         <v>312.84666666666669</v>
       </c>
-      <c r="F136" s="29" t="s">
+      <c r="F136" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G136" s="27">
+      <c r="G136" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4304,17 +4359,17 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D137" s="30">
+      <c r="D137" s="29">
         <v>321.89999999999998</v>
       </c>
       <c r="E137" s="7">
         <f t="shared" si="10"/>
         <v>317.14666666666665</v>
       </c>
-      <c r="F137" s="29" t="s">
+      <c r="F137" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G137" s="27">
+      <c r="G137" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4329,17 +4384,17 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D138" s="30">
+      <c r="D138" s="29">
         <v>328.3</v>
       </c>
       <c r="E138" s="7">
         <f t="shared" si="10"/>
         <v>323.54666666666668</v>
       </c>
-      <c r="F138" s="29" t="s">
+      <c r="F138" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G138" s="27">
+      <c r="G138" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4354,17 +4409,17 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D139" s="30">
+      <c r="D139" s="29">
         <v>433.2</v>
       </c>
       <c r="E139" s="7">
         <f t="shared" si="10"/>
         <v>428.44666666666666</v>
       </c>
-      <c r="F139" s="29" t="s">
+      <c r="F139" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G139" s="27">
+      <c r="G139" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4379,17 +4434,17 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D140" s="30">
+      <c r="D140" s="29">
         <v>309</v>
       </c>
       <c r="E140" s="7">
         <f t="shared" si="10"/>
         <v>304.24666666666667</v>
       </c>
-      <c r="F140" s="29" t="s">
+      <c r="F140" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G140" s="27">
+      <c r="G140" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4404,17 +4459,17 @@
         <f>$B$6</f>
         <v>4.753333333333333</v>
       </c>
-      <c r="D141" s="30">
+      <c r="D141" s="29">
         <v>333.5</v>
       </c>
       <c r="E141" s="7">
         <f t="shared" si="10"/>
         <v>328.74666666666667</v>
       </c>
-      <c r="F141" s="29" t="s">
+      <c r="F141" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G141" s="27">
+      <c r="G141" s="26">
         <v>41313</v>
       </c>
       <c r="H141" s="20"/>
@@ -4448,17 +4503,17 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D142" s="30">
+      <c r="D142" s="29">
         <v>394.3</v>
       </c>
       <c r="E142" s="7">
         <f t="shared" si="10"/>
         <v>389.54666666666668</v>
       </c>
-      <c r="F142" s="29" t="s">
+      <c r="F142" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G142" s="27">
+      <c r="G142" s="26">
         <v>41313</v>
       </c>
       <c r="H142" s="20"/>
@@ -4492,17 +4547,17 @@
         <f>$B$6</f>
         <v>4.753333333333333</v>
       </c>
-      <c r="D143" s="30">
+      <c r="D143" s="29">
         <v>418</v>
       </c>
       <c r="E143" s="7">
         <f t="shared" si="10"/>
         <v>413.24666666666667</v>
       </c>
-      <c r="F143" s="29" t="s">
+      <c r="F143" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G143" s="27">
+      <c r="G143" s="26">
         <v>41313</v>
       </c>
       <c r="H143" s="20"/>
@@ -4536,17 +4591,17 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D144" s="30">
+      <c r="D144" s="29">
         <v>448.6</v>
       </c>
       <c r="E144" s="7">
         <f t="shared" si="10"/>
         <v>443.84666666666669</v>
       </c>
-      <c r="F144" s="29" t="s">
+      <c r="F144" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G144" s="27">
+      <c r="G144" s="26">
         <v>41313</v>
       </c>
       <c r="H144" s="20"/>
@@ -4580,17 +4635,17 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D145" s="30">
+      <c r="D145" s="29">
         <v>332.2</v>
       </c>
       <c r="E145" s="7">
         <f t="shared" si="10"/>
         <v>327.44666666666666</v>
       </c>
-      <c r="F145" s="29" t="s">
+      <c r="F145" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G145" s="27">
+      <c r="G145" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4605,15 +4660,11 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D146" s="30"/>
-      <c r="E146" s="7">
-        <f t="shared" si="10"/>
-        <v>-4.753333333333333</v>
-      </c>
-      <c r="F146" s="29" t="s">
+      <c r="D146" s="29"/>
+      <c r="F146" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G146" s="27">
+      <c r="G146" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4628,15 +4679,11 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D147" s="30"/>
-      <c r="E147" s="7">
-        <f t="shared" si="10"/>
-        <v>-4.753333333333333</v>
-      </c>
-      <c r="F147" s="29" t="s">
+      <c r="D147" s="29"/>
+      <c r="F147" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G147" s="27">
+      <c r="G147" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4651,15 +4698,11 @@
         <f t="shared" si="11"/>
         <v>4.753333333333333</v>
       </c>
-      <c r="D148" s="30"/>
-      <c r="E148" s="7">
-        <f t="shared" si="10"/>
-        <v>-4.753333333333333</v>
-      </c>
-      <c r="F148" s="29" t="s">
+      <c r="D148" s="29"/>
+      <c r="F148" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G148" s="27">
+      <c r="G148" s="26">
         <v>41313</v>
       </c>
     </row>
@@ -4672,7 +4715,7 @@
       <c r="D149" s="15"/>
       <c r="E149" s="15">
         <f>SUM(E128:E148)</f>
-        <v>6527.6800000000012</v>
+        <v>6541.9400000000005</v>
       </c>
       <c r="F149" s="14"/>
       <c r="G149" s="14"/>
@@ -4697,32 +4740,32 @@
       <c r="Z149" s="14"/>
     </row>
     <row r="150" spans="1:26">
-      <c r="A150" s="23"/>
-      <c r="B150" s="23"/>
-      <c r="C150" s="24"/>
-      <c r="D150" s="23"/>
-      <c r="E150" s="23"/>
-      <c r="F150" s="23"/>
-      <c r="G150" s="24"/>
-      <c r="H150" s="25"/>
-      <c r="I150" s="25"/>
-      <c r="J150" s="25"/>
-      <c r="K150" s="24"/>
-      <c r="L150" s="25"/>
-      <c r="M150" s="25"/>
-      <c r="N150" s="25"/>
-      <c r="O150" s="23"/>
-      <c r="P150" s="24"/>
-      <c r="Q150" s="23"/>
-      <c r="R150" s="23"/>
-      <c r="S150" s="24"/>
-      <c r="T150" s="24"/>
-      <c r="U150" s="23"/>
-      <c r="V150" s="23"/>
-      <c r="W150" s="23"/>
-      <c r="X150" s="23"/>
-      <c r="Y150" s="23"/>
-      <c r="Z150" s="23"/>
+      <c r="A150" s="22"/>
+      <c r="B150" s="22"/>
+      <c r="C150" s="23"/>
+      <c r="D150" s="22"/>
+      <c r="E150" s="22"/>
+      <c r="F150" s="22"/>
+      <c r="G150" s="23"/>
+      <c r="H150" s="24"/>
+      <c r="I150" s="24"/>
+      <c r="J150" s="24"/>
+      <c r="K150" s="23"/>
+      <c r="L150" s="24"/>
+      <c r="M150" s="24"/>
+      <c r="N150" s="24"/>
+      <c r="O150" s="22"/>
+      <c r="P150" s="23"/>
+      <c r="Q150" s="22"/>
+      <c r="R150" s="22"/>
+      <c r="S150" s="23"/>
+      <c r="T150" s="23"/>
+      <c r="U150" s="22"/>
+      <c r="V150" s="22"/>
+      <c r="W150" s="22"/>
+      <c r="X150" s="22"/>
+      <c r="Y150" s="22"/>
+      <c r="Z150" s="22"/>
     </row>
     <row r="151" spans="1:26">
       <c r="A151" s="20" t="s">
@@ -4734,16 +4777,17 @@
       <c r="C151" s="21">
         <v>4.75</v>
       </c>
-      <c r="D151" s="31">
+      <c r="D151" s="30">
         <v>558.20000000000005</v>
       </c>
-      <c r="E151" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F151" s="28" t="s">
+      <c r="E151" s="7">
+        <f>D151-C151</f>
+        <v>553.45000000000005</v>
+      </c>
+      <c r="F151" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G151" s="27">
+      <c r="G151" s="26">
         <v>41313</v>
       </c>
       <c r="H151" s="20"/>
@@ -4776,16 +4820,17 @@
       <c r="C152" s="21">
         <v>4.75</v>
       </c>
-      <c r="D152" s="31">
+      <c r="D152" s="30">
         <v>535.1</v>
       </c>
-      <c r="E152" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F152" s="28" t="s">
+      <c r="E152" s="7">
+        <f>D152-C152</f>
+        <v>530.35</v>
+      </c>
+      <c r="F152" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G152" s="27">
+      <c r="G152" s="26">
         <v>41313</v>
       </c>
       <c r="H152" s="20"/>
@@ -4818,16 +4863,17 @@
       <c r="C153" s="21">
         <v>4.75</v>
       </c>
-      <c r="D153" s="31">
+      <c r="D153" s="30">
         <v>484.1</v>
       </c>
-      <c r="E153" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F153" s="28" t="s">
+      <c r="E153" s="7">
+        <f t="shared" ref="E153:E171" si="12">D153-C153</f>
+        <v>479.35</v>
+      </c>
+      <c r="F153" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G153" s="27">
+      <c r="G153" s="26">
         <v>41313</v>
       </c>
       <c r="H153" s="20"/>
@@ -4860,16 +4906,17 @@
       <c r="C154" s="21">
         <v>4.75</v>
       </c>
-      <c r="D154" s="31">
+      <c r="D154" s="30">
         <v>464.1</v>
       </c>
-      <c r="E154" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F154" s="28" t="s">
+      <c r="E154" s="7">
+        <f t="shared" si="12"/>
+        <v>459.35</v>
+      </c>
+      <c r="F154" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G154" s="27">
+      <c r="G154" s="26">
         <v>41313</v>
       </c>
       <c r="H154" s="20"/>
@@ -4902,16 +4949,17 @@
       <c r="C155" s="21">
         <v>4.75</v>
       </c>
-      <c r="D155" s="31">
+      <c r="D155" s="30">
         <v>450.1</v>
       </c>
-      <c r="E155" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F155" s="28" t="s">
+      <c r="E155" s="7">
+        <f t="shared" si="12"/>
+        <v>445.35</v>
+      </c>
+      <c r="F155" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G155" s="27">
+      <c r="G155" s="26">
         <v>41313</v>
       </c>
       <c r="H155" s="20"/>
@@ -4944,16 +4992,17 @@
       <c r="C156" s="21">
         <v>4.75</v>
       </c>
-      <c r="D156" s="31">
+      <c r="D156" s="30">
         <v>494.9</v>
       </c>
-      <c r="E156" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F156" s="28" t="s">
+      <c r="E156" s="7">
+        <f t="shared" si="12"/>
+        <v>490.15</v>
+      </c>
+      <c r="F156" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G156" s="27">
+      <c r="G156" s="26">
         <v>41313</v>
       </c>
       <c r="H156" s="20"/>
@@ -4986,16 +5035,17 @@
       <c r="C157" s="21">
         <v>4.75</v>
       </c>
-      <c r="D157" s="31">
+      <c r="D157" s="30">
         <v>393.5</v>
       </c>
-      <c r="E157" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F157" s="28" t="s">
+      <c r="E157" s="7">
+        <f t="shared" si="12"/>
+        <v>388.75</v>
+      </c>
+      <c r="F157" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G157" s="27">
+      <c r="G157" s="26">
         <v>41313</v>
       </c>
       <c r="H157" s="20"/>
@@ -5028,16 +5078,17 @@
       <c r="C158" s="21">
         <v>4.75</v>
       </c>
-      <c r="D158" s="31">
+      <c r="D158" s="30">
         <v>354.6</v>
       </c>
-      <c r="E158" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F158" s="28" t="s">
+      <c r="E158" s="7">
+        <f t="shared" si="12"/>
+        <v>349.85</v>
+      </c>
+      <c r="F158" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G158" s="27">
+      <c r="G158" s="26">
         <v>41313</v>
       </c>
       <c r="H158" s="20"/>
@@ -5070,16 +5121,17 @@
       <c r="C159" s="21">
         <v>4.75</v>
       </c>
-      <c r="D159" s="31">
+      <c r="D159" s="30">
         <v>475.4</v>
       </c>
-      <c r="E159" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F159" s="28" t="s">
+      <c r="E159" s="7">
+        <f t="shared" si="12"/>
+        <v>470.65</v>
+      </c>
+      <c r="F159" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G159" s="27">
+      <c r="G159" s="26">
         <v>41313</v>
       </c>
       <c r="H159" s="20"/>
@@ -5112,16 +5164,17 @@
       <c r="C160" s="21">
         <v>4.75</v>
       </c>
-      <c r="D160" s="31">
+      <c r="D160" s="30">
         <v>507.8</v>
       </c>
-      <c r="E160" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F160" s="28" t="s">
+      <c r="E160" s="7">
+        <f t="shared" si="12"/>
+        <v>503.05</v>
+      </c>
+      <c r="F160" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G160" s="27">
+      <c r="G160" s="26">
         <v>41313</v>
       </c>
       <c r="H160" s="20"/>
@@ -5154,16 +5207,17 @@
       <c r="C161" s="21">
         <v>4.75</v>
       </c>
-      <c r="D161" s="31">
+      <c r="D161" s="30">
         <v>536.5</v>
       </c>
-      <c r="E161" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F161" s="28" t="s">
+      <c r="E161" s="7">
+        <f t="shared" si="12"/>
+        <v>531.75</v>
+      </c>
+      <c r="F161" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G161" s="27">
+      <c r="G161" s="26">
         <v>41313</v>
       </c>
       <c r="H161" s="20"/>
@@ -5196,16 +5250,17 @@
       <c r="C162" s="21">
         <v>4.75</v>
       </c>
-      <c r="D162" s="31">
+      <c r="D162" s="30">
         <v>511</v>
       </c>
-      <c r="E162" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F162" s="28" t="s">
+      <c r="E162" s="7">
+        <f t="shared" si="12"/>
+        <v>506.25</v>
+      </c>
+      <c r="F162" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G162" s="27">
+      <c r="G162" s="26">
         <v>41313</v>
       </c>
       <c r="H162" s="20"/>
@@ -5238,16 +5293,17 @@
       <c r="C163" s="21">
         <v>4.75</v>
       </c>
-      <c r="D163" s="31">
+      <c r="D163" s="30">
         <v>350.7</v>
       </c>
-      <c r="E163" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F163" s="28" t="s">
+      <c r="E163" s="7">
+        <f t="shared" si="12"/>
+        <v>345.95</v>
+      </c>
+      <c r="F163" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G163" s="27">
+      <c r="G163" s="26">
         <v>41313</v>
       </c>
       <c r="H163" s="20"/>
@@ -5280,16 +5336,17 @@
       <c r="C164" s="21">
         <v>4.75</v>
       </c>
-      <c r="D164" s="31">
+      <c r="D164" s="30">
         <v>558.70000000000005</v>
       </c>
-      <c r="E164" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F164" s="28" t="s">
+      <c r="E164" s="7">
+        <f t="shared" si="12"/>
+        <v>553.95000000000005</v>
+      </c>
+      <c r="F164" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G164" s="27">
+      <c r="G164" s="26">
         <v>41313</v>
       </c>
       <c r="H164" s="20"/>
@@ -5322,16 +5379,17 @@
       <c r="C165" s="21">
         <v>4.75</v>
       </c>
-      <c r="D165" s="31">
+      <c r="D165" s="30">
         <v>365.4</v>
       </c>
-      <c r="E165" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F165" s="28" t="s">
+      <c r="E165" s="7">
+        <f t="shared" si="12"/>
+        <v>360.65</v>
+      </c>
+      <c r="F165" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G165" s="27">
+      <c r="G165" s="26">
         <v>41313</v>
       </c>
       <c r="H165" s="20"/>
@@ -5364,16 +5422,17 @@
       <c r="C166" s="21">
         <v>4.75</v>
       </c>
-      <c r="D166" s="31">
+      <c r="D166" s="30">
         <v>381.3</v>
       </c>
-      <c r="E166" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F166" s="28" t="s">
+      <c r="E166" s="7">
+        <f t="shared" si="12"/>
+        <v>376.55</v>
+      </c>
+      <c r="F166" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G166" s="27">
+      <c r="G166" s="26">
         <v>41313</v>
       </c>
       <c r="H166" s="20"/>
@@ -5406,16 +5465,17 @@
       <c r="C167" s="21">
         <v>4.75</v>
       </c>
-      <c r="D167" s="31">
+      <c r="D167" s="30">
         <v>510.4</v>
       </c>
-      <c r="E167" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F167" s="28" t="s">
+      <c r="E167" s="7">
+        <f t="shared" si="12"/>
+        <v>505.65</v>
+      </c>
+      <c r="F167" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G167" s="27">
+      <c r="G167" s="26">
         <v>41313</v>
       </c>
       <c r="H167" s="20"/>
@@ -5448,16 +5508,17 @@
       <c r="C168" s="21">
         <v>4.75</v>
       </c>
-      <c r="D168" s="31">
+      <c r="D168" s="30">
         <v>605.70000000000005</v>
       </c>
-      <c r="E168" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F168" s="28" t="s">
+      <c r="E168" s="7">
+        <f t="shared" si="12"/>
+        <v>600.95000000000005</v>
+      </c>
+      <c r="F168" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G168" s="27">
+      <c r="G168" s="26">
         <v>41313</v>
       </c>
       <c r="H168" s="20"/>
@@ -5490,16 +5551,17 @@
       <c r="C169" s="21">
         <v>4.75</v>
       </c>
-      <c r="D169" s="31">
+      <c r="D169" s="30">
         <v>557.4</v>
       </c>
-      <c r="E169" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F169" s="28" t="s">
+      <c r="E169" s="7">
+        <f t="shared" si="12"/>
+        <v>552.65</v>
+      </c>
+      <c r="F169" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G169" s="27">
+      <c r="G169" s="26">
         <v>41313</v>
       </c>
       <c r="H169" s="20"/>
@@ -5532,16 +5594,17 @@
       <c r="C170" s="21">
         <v>4.75</v>
       </c>
-      <c r="D170" s="31">
+      <c r="D170" s="30">
         <v>568.5</v>
       </c>
-      <c r="E170" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F170" s="28" t="s">
+      <c r="E170" s="7">
+        <f t="shared" si="12"/>
+        <v>563.75</v>
+      </c>
+      <c r="F170" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G170" s="27">
+      <c r="G170" s="26">
         <v>41313</v>
       </c>
       <c r="H170" s="20"/>
@@ -5574,16 +5637,17 @@
       <c r="C171" s="21">
         <v>4.75</v>
       </c>
-      <c r="D171" s="31">
+      <c r="D171" s="30">
         <v>434</v>
       </c>
-      <c r="E171" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F171" s="28" t="s">
+      <c r="E171" s="7">
+        <f t="shared" si="12"/>
+        <v>429.25</v>
+      </c>
+      <c r="F171" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="G171" s="27">
+      <c r="G171" s="26">
         <v>41313</v>
       </c>
       <c r="H171" s="20"/>
@@ -5614,7 +5678,8 @@
       <c r="C172" s="19"/>
       <c r="D172" s="15"/>
       <c r="E172" s="15">
-        <v>-99.8</v>
+        <f>SUM(E151:E171)</f>
+        <v>9997.65</v>
       </c>
       <c r="F172" s="14"/>
       <c r="G172" s="14"/>
@@ -5639,32 +5704,32 @@
       <c r="Z172" s="14"/>
     </row>
     <row r="173" spans="1:26">
-      <c r="A173" s="23"/>
-      <c r="B173" s="23"/>
-      <c r="C173" s="24"/>
-      <c r="D173" s="23"/>
-      <c r="E173" s="23"/>
-      <c r="F173" s="23"/>
-      <c r="G173" s="24"/>
-      <c r="H173" s="25"/>
-      <c r="I173" s="25"/>
-      <c r="J173" s="25"/>
-      <c r="K173" s="24"/>
-      <c r="L173" s="25"/>
-      <c r="M173" s="25"/>
-      <c r="N173" s="25"/>
-      <c r="O173" s="23"/>
-      <c r="P173" s="24"/>
-      <c r="Q173" s="23"/>
-      <c r="R173" s="23"/>
-      <c r="S173" s="24"/>
-      <c r="T173" s="24"/>
-      <c r="U173" s="23"/>
-      <c r="V173" s="23"/>
-      <c r="W173" s="23"/>
-      <c r="X173" s="23"/>
-      <c r="Y173" s="23"/>
-      <c r="Z173" s="23"/>
+      <c r="A173" s="22"/>
+      <c r="B173" s="22"/>
+      <c r="C173" s="23"/>
+      <c r="D173" s="22"/>
+      <c r="E173" s="22"/>
+      <c r="F173" s="22"/>
+      <c r="G173" s="23"/>
+      <c r="H173" s="24"/>
+      <c r="I173" s="24"/>
+      <c r="J173" s="24"/>
+      <c r="K173" s="23"/>
+      <c r="L173" s="24"/>
+      <c r="M173" s="24"/>
+      <c r="N173" s="24"/>
+      <c r="O173" s="22"/>
+      <c r="P173" s="23"/>
+      <c r="Q173" s="22"/>
+      <c r="R173" s="22"/>
+      <c r="S173" s="23"/>
+      <c r="T173" s="23"/>
+      <c r="U173" s="22"/>
+      <c r="V173" s="22"/>
+      <c r="W173" s="22"/>
+      <c r="X173" s="22"/>
+      <c r="Y173" s="22"/>
+      <c r="Z173" s="22"/>
     </row>
     <row r="174" spans="1:26">
       <c r="A174" s="20" t="s">
@@ -5676,16 +5741,17 @@
       <c r="C174" s="21">
         <v>4.75</v>
       </c>
-      <c r="D174" s="31">
+      <c r="D174" s="30">
         <v>339.3</v>
       </c>
-      <c r="E174" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F174" s="29" t="s">
+      <c r="E174" s="7">
+        <f>D174-C174</f>
+        <v>334.55</v>
+      </c>
+      <c r="F174" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G174" s="27">
+      <c r="G174" s="26">
         <v>41313</v>
       </c>
       <c r="H174" s="20"/>
@@ -5718,16 +5784,17 @@
       <c r="C175" s="21">
         <v>4.75</v>
       </c>
-      <c r="D175" s="31">
+      <c r="D175" s="30">
         <v>549.9</v>
       </c>
-      <c r="E175" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F175" s="29" t="s">
+      <c r="E175" s="7">
+        <f>D175-C175</f>
+        <v>545.15</v>
+      </c>
+      <c r="F175" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G175" s="27">
+      <c r="G175" s="26">
         <v>41313</v>
       </c>
       <c r="H175" s="20"/>
@@ -5760,16 +5827,17 @@
       <c r="C176" s="21">
         <v>4.75</v>
       </c>
-      <c r="D176" s="31">
+      <c r="D176" s="30">
         <v>389.5</v>
       </c>
-      <c r="E176" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F176" s="29" t="s">
+      <c r="E176" s="7">
+        <f t="shared" ref="E176:E185" si="13">D176-C176</f>
+        <v>384.75</v>
+      </c>
+      <c r="F176" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G176" s="27">
+      <c r="G176" s="26">
         <v>41313</v>
       </c>
       <c r="H176" s="20"/>
@@ -5802,16 +5870,17 @@
       <c r="C177" s="21">
         <v>4.75</v>
       </c>
-      <c r="D177" s="31">
+      <c r="D177" s="30">
         <v>450.3</v>
       </c>
-      <c r="E177" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F177" s="29" t="s">
+      <c r="E177" s="7">
+        <f t="shared" si="13"/>
+        <v>445.55</v>
+      </c>
+      <c r="F177" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G177" s="27">
+      <c r="G177" s="26">
         <v>41313</v>
       </c>
       <c r="H177" s="20"/>
@@ -5844,16 +5913,17 @@
       <c r="C178" s="21">
         <v>4.75</v>
       </c>
-      <c r="D178" s="31">
+      <c r="D178" s="30">
         <v>459</v>
       </c>
-      <c r="E178" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F178" s="29" t="s">
+      <c r="E178" s="7">
+        <f t="shared" si="13"/>
+        <v>454.25</v>
+      </c>
+      <c r="F178" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G178" s="27">
+      <c r="G178" s="26">
         <v>41313</v>
       </c>
       <c r="H178" s="20"/>
@@ -5886,16 +5956,17 @@
       <c r="C179" s="21">
         <v>4.75</v>
       </c>
-      <c r="D179" s="31">
+      <c r="D179" s="30">
         <v>498.3</v>
       </c>
-      <c r="E179" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F179" s="29" t="s">
+      <c r="E179" s="7">
+        <f t="shared" si="13"/>
+        <v>493.55</v>
+      </c>
+      <c r="F179" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G179" s="27">
+      <c r="G179" s="26">
         <v>41313</v>
       </c>
       <c r="H179" s="20"/>
@@ -5928,16 +5999,17 @@
       <c r="C180" s="21">
         <v>4.75</v>
       </c>
-      <c r="D180" s="31">
+      <c r="D180" s="30">
         <v>467.6</v>
       </c>
-      <c r="E180" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F180" s="29" t="s">
+      <c r="E180" s="7">
+        <f t="shared" si="13"/>
+        <v>462.85</v>
+      </c>
+      <c r="F180" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G180" s="27">
+      <c r="G180" s="26">
         <v>41313</v>
       </c>
       <c r="H180" s="20"/>
@@ -5970,16 +6042,17 @@
       <c r="C181" s="21">
         <v>4.75</v>
       </c>
-      <c r="D181" s="31">
+      <c r="D181" s="30">
         <v>312</v>
       </c>
-      <c r="E181" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F181" s="29" t="s">
+      <c r="E181" s="7">
+        <f t="shared" si="13"/>
+        <v>307.25</v>
+      </c>
+      <c r="F181" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G181" s="27">
+      <c r="G181" s="26">
         <v>41313</v>
       </c>
       <c r="H181" s="20"/>
@@ -6012,16 +6085,17 @@
       <c r="C182" s="21">
         <v>4.75</v>
       </c>
-      <c r="D182" s="31">
+      <c r="D182" s="30">
         <v>398.8</v>
       </c>
-      <c r="E182" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F182" s="29" t="s">
+      <c r="E182" s="7">
+        <f t="shared" si="13"/>
+        <v>394.05</v>
+      </c>
+      <c r="F182" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G182" s="27">
+      <c r="G182" s="26">
         <v>41313</v>
       </c>
       <c r="H182" s="20"/>
@@ -6054,16 +6128,17 @@
       <c r="C183" s="21">
         <v>4.75</v>
       </c>
-      <c r="D183" s="31">
+      <c r="D183" s="30">
         <v>287.89999999999998</v>
       </c>
-      <c r="E183" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F183" s="29" t="s">
+      <c r="E183" s="7">
+        <f t="shared" si="13"/>
+        <v>283.14999999999998</v>
+      </c>
+      <c r="F183" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G183" s="27">
+      <c r="G183" s="26">
         <v>41313</v>
       </c>
       <c r="H183" s="20"/>
@@ -6096,16 +6171,17 @@
       <c r="C184" s="21">
         <v>4.75</v>
       </c>
-      <c r="D184" s="31">
+      <c r="D184" s="30">
         <v>437.8</v>
       </c>
-      <c r="E184" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F184" s="29" t="s">
+      <c r="E184" s="7">
+        <f t="shared" si="13"/>
+        <v>433.05</v>
+      </c>
+      <c r="F184" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G184" s="27">
+      <c r="G184" s="26">
         <v>41313</v>
       </c>
       <c r="H184" s="20"/>
@@ -6138,16 +6214,17 @@
       <c r="C185" s="21">
         <v>4.75</v>
       </c>
-      <c r="D185" s="31">
+      <c r="D185" s="30">
         <v>314.10000000000002</v>
       </c>
-      <c r="E185" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F185" s="29" t="s">
+      <c r="E185" s="7">
+        <f t="shared" si="13"/>
+        <v>309.35000000000002</v>
+      </c>
+      <c r="F185" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G185" s="27">
+      <c r="G185" s="26">
         <v>41313</v>
       </c>
       <c r="H185" s="20"/>
@@ -6180,16 +6257,17 @@
       <c r="C186" s="21">
         <v>4.75</v>
       </c>
-      <c r="D186" s="31">
+      <c r="D186" s="30">
         <v>460.2</v>
       </c>
-      <c r="E186" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F186" s="29" t="s">
+      <c r="E186" s="7">
+        <f>D186-C186</f>
+        <v>455.45</v>
+      </c>
+      <c r="F186" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G186" s="27">
+      <c r="G186" s="26">
         <v>41313</v>
       </c>
       <c r="H186" s="20"/>
@@ -6222,16 +6300,17 @@
       <c r="C187" s="21">
         <v>4.75</v>
       </c>
-      <c r="D187" s="31">
+      <c r="D187" s="30">
         <v>386.3</v>
       </c>
-      <c r="E187" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F187" s="29" t="s">
+      <c r="E187" s="7">
+        <f>D187-C187</f>
+        <v>381.55</v>
+      </c>
+      <c r="F187" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G187" s="27">
+      <c r="G187" s="26">
         <v>41313</v>
       </c>
       <c r="H187" s="20"/>
@@ -6264,16 +6343,17 @@
       <c r="C188" s="21">
         <v>4.75</v>
       </c>
-      <c r="D188" s="31">
+      <c r="D188" s="30">
         <v>329.6</v>
       </c>
-      <c r="E188" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F188" s="29" t="s">
+      <c r="E188" s="7">
+        <f t="shared" ref="E188:E196" si="14">D188-C188</f>
+        <v>324.85000000000002</v>
+      </c>
+      <c r="F188" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G188" s="27">
+      <c r="G188" s="26">
         <v>41313</v>
       </c>
       <c r="H188" s="20"/>
@@ -6306,16 +6386,17 @@
       <c r="C189" s="21">
         <v>4.75</v>
       </c>
-      <c r="D189" s="31">
+      <c r="D189" s="30">
         <v>422.1</v>
       </c>
-      <c r="E189" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F189" s="29" t="s">
+      <c r="E189" s="7">
+        <f t="shared" si="14"/>
+        <v>417.35</v>
+      </c>
+      <c r="F189" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G189" s="27">
+      <c r="G189" s="26">
         <v>41313</v>
       </c>
       <c r="H189" s="20"/>
@@ -6348,16 +6429,17 @@
       <c r="C190" s="21">
         <v>4.75</v>
       </c>
-      <c r="D190" s="31">
+      <c r="D190" s="30">
         <v>359.1</v>
       </c>
-      <c r="E190" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F190" s="29" t="s">
+      <c r="E190" s="7">
+        <f t="shared" si="14"/>
+        <v>354.35</v>
+      </c>
+      <c r="F190" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G190" s="27">
+      <c r="G190" s="26">
         <v>41313</v>
       </c>
       <c r="H190" s="20"/>
@@ -6390,16 +6472,17 @@
       <c r="C191" s="21">
         <v>4.75</v>
       </c>
-      <c r="D191" s="31">
+      <c r="D191" s="30">
         <v>438.8</v>
       </c>
-      <c r="E191" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F191" s="29" t="s">
+      <c r="E191" s="7">
+        <f t="shared" si="14"/>
+        <v>434.05</v>
+      </c>
+      <c r="F191" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G191" s="27">
+      <c r="G191" s="26">
         <v>41313</v>
       </c>
       <c r="H191" s="20"/>
@@ -6432,16 +6515,17 @@
       <c r="C192" s="21">
         <v>4.75</v>
       </c>
-      <c r="D192" s="31">
+      <c r="D192" s="30">
         <v>398.8</v>
       </c>
-      <c r="E192" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F192" s="29" t="s">
+      <c r="E192" s="7">
+        <f t="shared" si="14"/>
+        <v>394.05</v>
+      </c>
+      <c r="F192" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G192" s="27">
+      <c r="G192" s="26">
         <v>41313</v>
       </c>
       <c r="H192" s="20"/>
@@ -6474,16 +6558,17 @@
       <c r="C193" s="21">
         <v>4.75</v>
       </c>
-      <c r="D193" s="31">
+      <c r="D193" s="30">
         <v>355.7</v>
       </c>
-      <c r="E193" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F193" s="29" t="s">
+      <c r="E193" s="7">
+        <f t="shared" si="14"/>
+        <v>350.95</v>
+      </c>
+      <c r="F193" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G193" s="27">
+      <c r="G193" s="26">
         <v>41313</v>
       </c>
       <c r="H193" s="20"/>
@@ -6516,16 +6601,17 @@
       <c r="C194" s="21">
         <v>4.75</v>
       </c>
-      <c r="D194" s="31">
+      <c r="D194" s="30">
         <v>448.6</v>
       </c>
-      <c r="E194" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F194" s="29" t="s">
+      <c r="E194" s="7">
+        <f t="shared" si="14"/>
+        <v>443.85</v>
+      </c>
+      <c r="F194" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G194" s="27">
+      <c r="G194" s="26">
         <v>41313</v>
       </c>
       <c r="H194" s="20"/>
@@ -6558,16 +6644,17 @@
       <c r="C195" s="21">
         <v>4.75</v>
       </c>
-      <c r="D195" s="31">
+      <c r="D195" s="30">
         <v>339.8</v>
       </c>
-      <c r="E195" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F195" s="29" t="s">
+      <c r="E195" s="7">
+        <f t="shared" si="14"/>
+        <v>335.05</v>
+      </c>
+      <c r="F195" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G195" s="27">
+      <c r="G195" s="26">
         <v>41313</v>
       </c>
       <c r="H195" s="20"/>
@@ -6600,16 +6687,17 @@
       <c r="C196" s="21">
         <v>4.75</v>
       </c>
-      <c r="D196" s="31">
+      <c r="D196" s="30">
         <v>530.1</v>
       </c>
-      <c r="E196" s="22">
-        <v>-4.8</v>
-      </c>
-      <c r="F196" s="29" t="s">
+      <c r="E196" s="7">
+        <f>D196-C196</f>
+        <v>525.35</v>
+      </c>
+      <c r="F196" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="G196" s="27">
+      <c r="G196" s="26">
         <v>41313</v>
       </c>
       <c r="H196" s="20"/>
@@ -6640,7 +6728,8 @@
       <c r="C197" s="19"/>
       <c r="D197" s="15"/>
       <c r="E197" s="15">
-        <v>-99.8</v>
+        <f>SUM(E174:E196)</f>
+        <v>9264.3500000000022</v>
       </c>
       <c r="F197" s="14"/>
       <c r="G197" s="14"/>
@@ -6736,14 +6825,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">

</xml_diff>